<commit_message>
tlt-2426: refactors course info add people selenium tests, course info selenium test page objects, pulls updated version of selenium_common with api helper fix
</commit_message>
<xml_diff>
--- a/selenium_tests/course_info/test_data/admin_console_roles.xlsx
+++ b/selenium_tests/course_info/test_data/admin_console_roles.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ely817/tlt/canvas_account_admin_tools/selenium_tests/course_info/test_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>test_case_id</t>
   </si>
@@ -242,6 +247,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -570,15 +580,15 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -592,7 +602,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -606,154 +616,85 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="D4" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="1">
-        <v>15</v>
-      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -765,12 +706,12 @@
       <selection activeCell="C9" sqref="A1:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -784,7 +725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -798,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -812,7 +753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -826,7 +767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -840,7 +781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -854,7 +795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -868,7 +809,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -882,7 +823,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -896,7 +837,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -910,7 +851,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -924,7 +865,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -941,10 +882,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Added @ddt to course_info_remove_people_tests - updated admin_console_roles for Teaching Fellow to TA
</commit_message>
<xml_diff>
--- a/selenium_tests/course_info/test_data/admin_console_roles.xlsx
+++ b/selenium_tests/course_info/test_data/admin_console_roles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -118,9 +118,6 @@
     <t>Student</t>
   </si>
   <si>
-    <t>Teaching Fellow</t>
-  </si>
-  <si>
     <t>Designer</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>Observer</t>
+  </si>
+  <si>
+    <t>TA</t>
   </si>
 </sst>
 </file>
@@ -186,8 +186,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -215,7 +221,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -227,6 +233,9 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -238,6 +247,9 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -570,7 +582,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -642,7 +654,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1">
         <v>5</v>
@@ -656,7 +668,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1">
         <v>7</v>
@@ -712,7 +724,7 @@
         <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1">
         <v>12</v>
@@ -726,7 +738,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1">
         <v>14</v>
@@ -740,7 +752,7 @@
         <v>29</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1">
         <v>15</v>
@@ -762,7 +774,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="A1:D12"/>
+      <selection sqref="A1:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -834,7 +846,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1">
         <v>5</v>
@@ -848,7 +860,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1">
         <v>7</v>
@@ -904,7 +916,7 @@
         <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1">
         <v>12</v>
@@ -918,7 +930,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1">
         <v>14</v>
@@ -932,7 +944,7 @@
         <v>29</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1">
         <v>15</v>

</xml_diff>